<commit_message>
Full integration of caching feature [Final Commit?]
- integrated aengl5337's data caching feature preventing downloading new
  data if up to date data already exists.

- build_exe.py now copies the DATA folder alongside wb_list.xlsx into
  the distribution folder, so cached FAA/DCS/flight/fuel/comment data
  ships with the exe (stale data is auto-refreshed on first run via
  Alec's CycleCache cycle-date comparison)

- minor bug fixes.
</commit_message>
<xml_diff>
--- a/wb_list.xlsx
+++ b/wb_list.xlsx
@@ -867,12 +867,12 @@
       </c>
       <c r="Q2" s="19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R2" s="19" t="inlineStr">
         <is>
-          <t>BOW</t>
+          <t>CJO</t>
         </is>
       </c>
       <c r="S2" s="19" t="inlineStr">
@@ -954,17 +954,17 @@
       </c>
       <c r="Q3" s="19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R3" s="19" t="inlineStr">
         <is>
-          <t>JWG</t>
+          <t>CJO</t>
         </is>
       </c>
       <c r="S3" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="T3" s="19" t="n"/>
@@ -1022,17 +1022,17 @@
       </c>
       <c r="Q4" s="19" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R4" s="19" t="inlineStr">
         <is>
+          <t>CJO</t>
+        </is>
+      </c>
+      <c r="S4" s="19" t="inlineStr">
+        <is>
           <t>CMC</t>
-        </is>
-      </c>
-      <c r="S4" s="19" t="inlineStr">
-        <is>
-          <t>PRT</t>
         </is>
       </c>
       <c r="T4" s="19" t="n"/>
@@ -1090,17 +1090,17 @@
       </c>
       <c r="Q5" s="19" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R5" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>AFU</t>
         </is>
       </c>
       <c r="S5" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="T5" s="19" t="n"/>
@@ -1158,16 +1158,18 @@
       </c>
       <c r="Q6" s="19" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R6" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
-        </is>
-      </c>
-      <c r="S6" s="19" t="n">
-        <v/>
+          <t>HAS</t>
+        </is>
+      </c>
+      <c r="S6" s="19" t="inlineStr">
+        <is>
+          <t>WSM</t>
+        </is>
       </c>
       <c r="T6" s="19" t="n"/>
       <c r="U6" s="19" t="inlineStr">
@@ -1225,17 +1227,17 @@
       </c>
       <c r="Q7" s="19" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R7" s="19" t="inlineStr">
         <is>
-          <t>JPJ</t>
+          <t>HAS</t>
         </is>
       </c>
       <c r="S7" s="19" t="inlineStr">
         <is>
-          <t>WLS</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="T7" s="19" t="n"/>
@@ -1294,17 +1296,17 @@
       </c>
       <c r="Q8" s="19" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R8" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S8" s="19" t="inlineStr">
         <is>
-          <t>FRU</t>
+          <t>JWA</t>
         </is>
       </c>
       <c r="T8" s="19" t="n"/>
@@ -1358,18 +1360,16 @@
       </c>
       <c r="Q9" s="19" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R9" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
-        </is>
-      </c>
-      <c r="S9" s="19" t="inlineStr">
-        <is>
-          <t>JAM</t>
-        </is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S9" s="19" t="n">
+        <v/>
       </c>
       <c r="T9" s="19" t="n"/>
       <c r="U9" s="19" t="n"/>
@@ -1419,18 +1419,16 @@
       </c>
       <c r="Q10" s="19" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R10" s="19" t="inlineStr">
         <is>
-          <t>ADO</t>
-        </is>
-      </c>
-      <c r="S10" s="19" t="inlineStr">
-        <is>
-          <t>HAS</t>
-        </is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S10" s="19" t="n">
+        <v/>
       </c>
       <c r="T10" s="19" t="n"/>
       <c r="U10" s="19" t="n"/>
@@ -1476,17 +1474,17 @@
       </c>
       <c r="Q11" s="19" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R11" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S11" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
+          <t>RBL</t>
         </is>
       </c>
       <c r="T11" s="19" t="n"/>
@@ -1534,17 +1532,17 @@
       </c>
       <c r="Q12" s="19" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R12" s="19" t="inlineStr">
         <is>
-          <t>BAM</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S12" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>RBL</t>
         </is>
       </c>
       <c r="T12" s="19" t="n"/>
@@ -1596,17 +1594,17 @@
       </c>
       <c r="Q13" s="19" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="R13" s="19" t="inlineStr">
         <is>
-          <t>KCO</t>
+          <t>CBI</t>
         </is>
       </c>
       <c r="S13" s="19" t="inlineStr">
         <is>
-          <t>MBE</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="T13" s="19" t="n"/>
@@ -1653,17 +1651,17 @@
       </c>
       <c r="Q14" s="19" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="R14" s="19" t="inlineStr">
         <is>
-          <t>ADO</t>
+          <t>JWG</t>
         </is>
       </c>
       <c r="S14" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="T14" s="19" t="n"/>
@@ -1706,17 +1704,17 @@
       </c>
       <c r="Q15" s="19" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="R15" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="S15" s="19" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="T15" s="19" t="n"/>
@@ -1759,18 +1757,16 @@
       </c>
       <c r="Q16" s="19" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="R16" s="19" t="inlineStr">
         <is>
-          <t>JWA</t>
-        </is>
-      </c>
-      <c r="S16" s="19" t="inlineStr">
-        <is>
-          <t>MAN</t>
-        </is>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S16" s="19" t="n">
+        <v/>
       </c>
       <c r="T16" s="19" t="n"/>
       <c r="U16" s="19" t="n"/>
@@ -1813,17 +1809,17 @@
       </c>
       <c r="Q17" s="19" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="R17" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>JPJ</t>
         </is>
       </c>
       <c r="S17" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>WLS</t>
         </is>
       </c>
       <c r="T17" s="19" t="n"/>
@@ -1871,17 +1867,17 @@
       </c>
       <c r="Q18" s="19" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="R18" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>HMK</t>
         </is>
       </c>
       <c r="S18" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="T18" s="19" t="n"/>
@@ -1924,17 +1920,17 @@
       </c>
       <c r="Q19" s="19" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="R19" s="19" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>ADO</t>
         </is>
       </c>
       <c r="S19" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="T19" s="19" t="n"/>
@@ -1977,17 +1973,17 @@
       </c>
       <c r="Q20" s="19" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="R20" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S20" s="19" t="inlineStr">
         <is>
-          <t>HMK</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="T20" s="19" t="n"/>
@@ -2031,17 +2027,17 @@
       </c>
       <c r="Q21" s="19" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="R21" s="19" t="inlineStr">
         <is>
-          <t>JMO</t>
+          <t>JWA</t>
         </is>
       </c>
       <c r="S21" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="T21" s="19" t="n"/>
@@ -2089,17 +2085,17 @@
       </c>
       <c r="Q22" s="19" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="R22" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>CBI</t>
         </is>
       </c>
       <c r="S22" s="19" t="inlineStr">
         <is>
-          <t>JMO</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="T22" s="19" t="n"/>
@@ -2142,17 +2138,17 @@
       </c>
       <c r="Q23" s="19" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="R23" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>CBI</t>
         </is>
       </c>
       <c r="S23" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="T23" s="19" t="n"/>
@@ -2196,7 +2192,7 @@
       </c>
       <c r="Q24" s="19" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="R24" s="19" t="inlineStr">
@@ -2206,7 +2202,7 @@
       </c>
       <c r="S24" s="19" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="T24" s="19" t="n"/>
@@ -2254,17 +2250,17 @@
       </c>
       <c r="Q25" s="19" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="R25" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S25" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>HMK</t>
         </is>
       </c>
       <c r="T25" s="19" t="n"/>
@@ -2307,16 +2303,18 @@
       </c>
       <c r="Q26" s="19" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="R26" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="S26" s="19" t="n">
-        <v/>
+          <t>JMO</t>
+        </is>
+      </c>
+      <c r="S26" s="19" t="inlineStr">
+        <is>
+          <t>RJC</t>
+        </is>
       </c>
       <c r="T26" s="19" t="n"/>
       <c r="U26" s="19" t="n"/>
@@ -2359,7 +2357,7 @@
       </c>
       <c r="Q27" s="19" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="R27" s="19" t="inlineStr">
@@ -2369,7 +2367,7 @@
       </c>
       <c r="S27" s="19" t="inlineStr">
         <is>
-          <t>FRU</t>
+          <t>LOV</t>
         </is>
       </c>
       <c r="T27" s="19" t="n"/>
@@ -2413,17 +2411,17 @@
       </c>
       <c r="Q28" s="19" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="R28" s="19" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="S28" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>TIN</t>
         </is>
       </c>
       <c r="T28" s="19" t="n"/>
@@ -2467,17 +2465,17 @@
       </c>
       <c r="Q29" s="19" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="R29" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>CBI</t>
         </is>
       </c>
       <c r="S29" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="T29" s="19" t="n"/>
@@ -2521,12 +2519,12 @@
       </c>
       <c r="Q30" s="19" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-19</t>
         </is>
       </c>
       <c r="R30" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="S30" s="19" t="n">
@@ -2573,17 +2571,17 @@
       </c>
       <c r="Q31" s="19" t="inlineStr">
         <is>
-          <t>2025-11-05</t>
+          <t>2025-11-19</t>
         </is>
       </c>
       <c r="R31" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S31" s="19" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="T31" s="19" t="n"/>
@@ -2615,17 +2613,17 @@
       </c>
       <c r="Q32" s="19" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-14</t>
         </is>
       </c>
       <c r="R32" s="19" t="inlineStr">
         <is>
-          <t>DAR</t>
+          <t>LAO</t>
         </is>
       </c>
       <c r="S32" s="19" t="inlineStr">
         <is>
-          <t>RTH</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="T32" s="19" t="n"/>
@@ -2657,16 +2655,18 @@
       </c>
       <c r="Q33" s="19" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="R33" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S33" s="19" t="n">
-        <v/>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S33" s="19" t="inlineStr">
+        <is>
+          <t>LOV</t>
+        </is>
       </c>
       <c r="T33" s="19" t="n"/>
       <c r="U33" s="19" t="n"/>
@@ -2697,12 +2697,12 @@
       </c>
       <c r="Q34" s="19" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="R34" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S34" s="19" t="n">
@@ -2737,16 +2737,18 @@
       </c>
       <c r="Q35" s="19" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-11-05</t>
         </is>
       </c>
       <c r="R35" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S35" s="19" t="n">
-        <v/>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S35" s="19" t="inlineStr">
+        <is>
+          <t>BNE</t>
+        </is>
       </c>
       <c r="T35" s="19" t="n"/>
       <c r="U35" s="19" t="n"/>
@@ -2777,16 +2779,18 @@
       </c>
       <c r="Q36" s="19" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="R36" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
-        </is>
-      </c>
-      <c r="S36" s="19" t="n">
-        <v/>
+          <t>DAR</t>
+        </is>
+      </c>
+      <c r="S36" s="19" t="inlineStr">
+        <is>
+          <t>RTH</t>
+        </is>
       </c>
       <c r="T36" s="19" t="n"/>
       <c r="U36" s="19" t="n"/>
@@ -2817,18 +2821,16 @@
       </c>
       <c r="Q37" s="19" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="R37" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
-        </is>
-      </c>
-      <c r="S37" s="19" t="inlineStr">
-        <is>
-          <t>FRU</t>
-        </is>
+          <t>DDC</t>
+        </is>
+      </c>
+      <c r="S37" s="19" t="n">
+        <v/>
       </c>
       <c r="T37" s="19" t="n"/>
       <c r="U37" s="19" t="n"/>
@@ -2859,7 +2861,7 @@
       </c>
       <c r="Q38" s="19" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="R38" s="19" t="inlineStr">
@@ -2867,10 +2869,8 @@
           <t>DDC</t>
         </is>
       </c>
-      <c r="S38" s="19" t="inlineStr">
-        <is>
-          <t>LOV</t>
-        </is>
+      <c r="S38" s="19" t="n">
+        <v/>
       </c>
       <c r="T38" s="19" t="n"/>
       <c r="U38" s="19" t="n"/>
@@ -2901,18 +2901,16 @@
       </c>
       <c r="Q39" s="19" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="R39" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S39" s="19" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
+          <t>DDC</t>
+        </is>
+      </c>
+      <c r="S39" s="19" t="n">
+        <v/>
       </c>
       <c r="T39" s="19" t="n"/>
       <c r="U39" s="19" t="n"/>
@@ -2943,18 +2941,16 @@
       </c>
       <c r="Q40" s="19" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="R40" s="19" t="inlineStr">
         <is>
-          <t>AML</t>
-        </is>
-      </c>
-      <c r="S40" s="19" t="inlineStr">
-        <is>
-          <t>SMB</t>
-        </is>
+          <t>GLO</t>
+        </is>
+      </c>
+      <c r="S40" s="19" t="n">
+        <v/>
       </c>
       <c r="T40" s="19" t="n"/>
       <c r="U40" s="19" t="n"/>
@@ -2985,17 +2981,17 @@
       </c>
       <c r="Q41" s="19" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="R41" s="19" t="inlineStr">
         <is>
-          <t>AML</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="S41" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="T41" s="19" t="n"/>
@@ -3027,16 +3023,18 @@
       </c>
       <c r="Q42" s="19" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="R42" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
-        </is>
-      </c>
-      <c r="S42" s="19" t="n">
-        <v/>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S42" s="19" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
       </c>
       <c r="T42" s="19" t="n"/>
       <c r="U42" s="19" t="n"/>
@@ -3067,17 +3065,17 @@
       </c>
       <c r="Q43" s="19" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="R43" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>AML</t>
         </is>
       </c>
       <c r="S43" s="19" t="inlineStr">
         <is>
-          <t>MBE</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="T43" s="19" t="n"/>
@@ -3109,17 +3107,17 @@
       </c>
       <c r="Q44" s="19" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="R44" s="19" t="inlineStr">
         <is>
-          <t>PWF</t>
+          <t>AML</t>
         </is>
       </c>
       <c r="S44" s="19" t="inlineStr">
         <is>
-          <t>RTH</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="T44" s="19" t="n"/>
@@ -3151,18 +3149,16 @@
       </c>
       <c r="Q45" s="19" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="R45" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S45" s="19" t="inlineStr">
-        <is>
-          <t>TIN</t>
-        </is>
+          <t>RJC</t>
+        </is>
+      </c>
+      <c r="S45" s="19" t="n">
+        <v/>
       </c>
       <c r="T45" s="19" t="n"/>
       <c r="U45" s="19" t="n"/>
@@ -3193,17 +3189,17 @@
       </c>
       <c r="Q46" s="19" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="R46" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="S46" s="19" t="inlineStr">
         <is>
-          <t>KCO</t>
+          <t>MBE</t>
         </is>
       </c>
       <c r="T46" s="19" t="n"/>
@@ -3235,17 +3231,17 @@
       </c>
       <c r="Q47" s="19" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="R47" s="19" t="inlineStr">
         <is>
-          <t>JWA</t>
+          <t>PWF</t>
         </is>
       </c>
       <c r="S47" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>RTH</t>
         </is>
       </c>
       <c r="T47" s="19" t="n"/>
@@ -3277,16 +3273,18 @@
       </c>
       <c r="Q48" s="19" t="inlineStr">
         <is>
-          <t>2025-08-03</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="R48" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
-        </is>
-      </c>
-      <c r="S48" s="19" t="n">
-        <v/>
+          <t>MBE</t>
+        </is>
+      </c>
+      <c r="S48" s="19" t="inlineStr">
+        <is>
+          <t>RJC</t>
+        </is>
       </c>
       <c r="T48" s="19" t="n"/>
       <c r="U48" s="19" t="n"/>
@@ -3317,16 +3315,18 @@
       </c>
       <c r="Q49" s="19" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-09-03</t>
         </is>
       </c>
       <c r="R49" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
-        </is>
-      </c>
-      <c r="S49" s="19" t="n">
-        <v/>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S49" s="19" t="inlineStr">
+        <is>
+          <t>KCO</t>
+        </is>
       </c>
       <c r="T49" s="19" t="n"/>
       <c r="U49" s="19" t="n"/>
@@ -3357,16 +3357,18 @@
       </c>
       <c r="Q50" s="19" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-22</t>
         </is>
       </c>
       <c r="R50" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
-        </is>
-      </c>
-      <c r="S50" s="19" t="n">
-        <v/>
+          <t>JWA</t>
+        </is>
+      </c>
+      <c r="S50" s="19" t="inlineStr">
+        <is>
+          <t>LDE</t>
+        </is>
       </c>
       <c r="T50" s="19" t="n"/>
       <c r="U50" s="19" t="n"/>
@@ -3397,18 +3399,16 @@
       </c>
       <c r="Q51" s="19" t="inlineStr">
         <is>
-          <t>2025-07-10</t>
+          <t>2025-08-03</t>
         </is>
       </c>
       <c r="R51" s="19" t="inlineStr">
         <is>
-          <t>ADO</t>
-        </is>
-      </c>
-      <c r="S51" s="19" t="inlineStr">
-        <is>
-          <t>HAS</t>
-        </is>
+          <t>BAP</t>
+        </is>
+      </c>
+      <c r="S51" s="19" t="n">
+        <v/>
       </c>
       <c r="T51" s="19" t="n"/>
       <c r="U51" s="19" t="n"/>
@@ -3439,12 +3439,12 @@
       </c>
       <c r="Q52" s="19" t="inlineStr">
         <is>
-          <t>2025-07-06</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="R52" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="S52" s="19" t="n">
@@ -3479,12 +3479,12 @@
       </c>
       <c r="Q53" s="19" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="R53" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="S53" s="19" t="n">
@@ -3519,17 +3519,17 @@
       </c>
       <c r="Q54" s="19" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-10</t>
         </is>
       </c>
       <c r="R54" s="19" t="inlineStr">
         <is>
-          <t>HMK</t>
+          <t>ADO</t>
         </is>
       </c>
       <c r="S54" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>HAS</t>
         </is>
       </c>
       <c r="T54" s="19" t="n"/>
@@ -3561,18 +3561,16 @@
       </c>
       <c r="Q55" s="19" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-06</t>
         </is>
       </c>
       <c r="R55" s="19" t="inlineStr">
         <is>
-          <t>HMK</t>
-        </is>
-      </c>
-      <c r="S55" s="19" t="inlineStr">
-        <is>
-          <t>MAN</t>
-        </is>
+          <t>DDC</t>
+        </is>
+      </c>
+      <c r="S55" s="19" t="n">
+        <v/>
       </c>
       <c r="T55" s="19" t="n"/>
       <c r="U55" s="19" t="n"/>
@@ -3603,18 +3601,16 @@
       </c>
       <c r="Q56" s="19" t="inlineStr">
         <is>
-          <t>2025-06-30</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="R56" s="19" t="inlineStr">
         <is>
-          <t>CWI</t>
-        </is>
-      </c>
-      <c r="S56" s="19" t="inlineStr">
-        <is>
-          <t>SMB</t>
-        </is>
+          <t>DDC</t>
+        </is>
+      </c>
+      <c r="S56" s="19" t="n">
+        <v/>
       </c>
       <c r="T56" s="19" t="n"/>
       <c r="U56" s="19" t="n"/>
@@ -3645,16 +3641,18 @@
       </c>
       <c r="Q57" s="19" t="inlineStr">
         <is>
-          <t>2025-06-22</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="R57" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
-        </is>
-      </c>
-      <c r="S57" s="19" t="n">
-        <v/>
+          <t>HMK</t>
+        </is>
+      </c>
+      <c r="S57" s="19" t="inlineStr">
+        <is>
+          <t>MAN</t>
+        </is>
       </c>
       <c r="T57" s="19" t="n"/>
       <c r="U57" s="19" t="n"/>
@@ -3685,17 +3683,17 @@
       </c>
       <c r="Q58" s="19" t="inlineStr">
         <is>
-          <t>2025-06-20</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="R58" s="19" t="inlineStr">
         <is>
-          <t>JHA</t>
+          <t>HMK</t>
         </is>
       </c>
       <c r="S58" s="19" t="inlineStr">
         <is>
-          <t>MIR</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="T58" s="19" t="n"/>
@@ -3727,16 +3725,18 @@
       </c>
       <c r="Q59" s="19" t="inlineStr">
         <is>
-          <t>2025-06-15</t>
+          <t>2025-06-30</t>
         </is>
       </c>
       <c r="R59" s="19" t="inlineStr">
         <is>
+          <t>CWI</t>
+        </is>
+      </c>
+      <c r="S59" s="19" t="inlineStr">
+        <is>
           <t>SMB</t>
         </is>
-      </c>
-      <c r="S59" s="19" t="n">
-        <v/>
       </c>
       <c r="T59" s="19" t="n"/>
       <c r="U59" s="19" t="n"/>
@@ -3767,12 +3767,12 @@
       </c>
       <c r="Q60" s="19" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-06-22</t>
         </is>
       </c>
       <c r="R60" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="S60" s="19" t="n">
@@ -3807,17 +3807,17 @@
       </c>
       <c r="Q61" s="19" t="inlineStr">
         <is>
-          <t>2025-06-09</t>
+          <t>2025-06-20</t>
         </is>
       </c>
       <c r="R61" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>JHA</t>
         </is>
       </c>
       <c r="S61" s="19" t="inlineStr">
         <is>
-          <t>WLS</t>
+          <t>MIR</t>
         </is>
       </c>
       <c r="T61" s="19" t="n"/>
@@ -3849,18 +3849,16 @@
       </c>
       <c r="Q62" s="19" t="inlineStr">
         <is>
-          <t>2025-06-04</t>
+          <t>2025-06-15</t>
         </is>
       </c>
       <c r="R62" s="19" t="inlineStr">
         <is>
-          <t>MBE</t>
-        </is>
-      </c>
-      <c r="S62" s="19" t="inlineStr">
-        <is>
-          <t>RJC</t>
-        </is>
+          <t>SMB</t>
+        </is>
+      </c>
+      <c r="S62" s="19" t="n">
+        <v/>
       </c>
       <c r="T62" s="19" t="n"/>
       <c r="U62" s="19" t="n"/>
@@ -3891,7 +3889,7 @@
       </c>
       <c r="Q63" s="19" t="inlineStr">
         <is>
-          <t>2025-05-23</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="R63" s="19" t="inlineStr">
@@ -3931,16 +3929,18 @@
       </c>
       <c r="Q64" s="19" t="inlineStr">
         <is>
-          <t>2025-05-21</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="R64" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
-        </is>
-      </c>
-      <c r="S64" s="19" t="n">
-        <v/>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S64" s="19" t="inlineStr">
+        <is>
+          <t>WLS</t>
+        </is>
       </c>
       <c r="T64" s="19" t="n"/>
       <c r="U64" s="19" t="n"/>
@@ -3971,16 +3971,18 @@
       </c>
       <c r="Q65" s="19" t="inlineStr">
         <is>
-          <t>2025-05-21</t>
+          <t>2025-06-04</t>
         </is>
       </c>
       <c r="R65" s="19" t="inlineStr">
         <is>
+          <t>MBE</t>
+        </is>
+      </c>
+      <c r="S65" s="19" t="inlineStr">
+        <is>
           <t>RJC</t>
         </is>
-      </c>
-      <c r="S65" s="19" t="n">
-        <v/>
       </c>
       <c r="T65" s="19" t="n"/>
       <c r="U65" s="19" t="n"/>
@@ -4011,16 +4013,18 @@
       </c>
       <c r="Q66" s="19" t="inlineStr">
         <is>
-          <t>2025-05-21</t>
+          <t>2025-05-23</t>
         </is>
       </c>
       <c r="R66" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="S66" s="19" t="n">
-        <v/>
+          <t>JWG</t>
+        </is>
+      </c>
+      <c r="S66" s="19" t="inlineStr">
+        <is>
+          <t>SMB</t>
+        </is>
       </c>
       <c r="T66" s="19" t="n"/>
       <c r="U66" s="19" t="n"/>
@@ -4051,12 +4055,12 @@
       </c>
       <c r="Q67" s="19" t="inlineStr">
         <is>
-          <t>2025-04-23</t>
+          <t>2025-05-21</t>
         </is>
       </c>
       <c r="R67" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="S67" s="19" t="n">
@@ -4091,12 +4095,12 @@
       </c>
       <c r="Q68" s="19" t="inlineStr">
         <is>
-          <t>2025-04-20</t>
+          <t>2025-05-21</t>
         </is>
       </c>
       <c r="R68" s="19" t="inlineStr">
         <is>
-          <t>HAS</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="S68" s="19" t="n">
@@ -4131,12 +4135,12 @@
       </c>
       <c r="Q69" s="19" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-05-21</t>
         </is>
       </c>
       <c r="R69" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="S69" s="19" t="n">
@@ -4171,7 +4175,7 @@
       </c>
       <c r="Q70" s="19" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="R70" s="19" t="inlineStr">
@@ -4211,12 +4215,12 @@
       </c>
       <c r="Q71" s="19" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-20</t>
         </is>
       </c>
       <c r="R71" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>HAS</t>
         </is>
       </c>
       <c r="S71" s="19" t="n">
@@ -4251,12 +4255,12 @@
       </c>
       <c r="Q72" s="19" t="inlineStr">
         <is>
-          <t>2025-03-11</t>
+          <t>2025-04-19</t>
         </is>
       </c>
       <c r="R72" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S72" s="19" t="n">
@@ -4291,7 +4295,7 @@
       </c>
       <c r="Q73" s="19" t="inlineStr">
         <is>
-          <t>2024-11-21</t>
+          <t>2025-04-19</t>
         </is>
       </c>
       <c r="R73" s="19" t="inlineStr">
@@ -4331,7 +4335,7 @@
       </c>
       <c r="Q74" s="19" t="inlineStr">
         <is>
-          <t>2024-11-21</t>
+          <t>2025-04-19</t>
         </is>
       </c>
       <c r="R74" s="19" t="inlineStr">
@@ -4371,12 +4375,12 @@
       </c>
       <c r="Q75" s="19" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
+          <t>2025-03-11</t>
         </is>
       </c>
       <c r="R75" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="S75" s="19" t="n">
@@ -4411,18 +4415,16 @@
       </c>
       <c r="Q76" s="19" t="inlineStr">
         <is>
-          <t>2024-11-07</t>
+          <t>2024-11-21</t>
         </is>
       </c>
       <c r="R76" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
-        </is>
-      </c>
-      <c r="S76" s="19" t="inlineStr">
-        <is>
-          <t>JAM</t>
-        </is>
+          <t>GLO</t>
+        </is>
+      </c>
+      <c r="S76" s="19" t="n">
+        <v/>
       </c>
       <c r="T76" s="19" t="n"/>
       <c r="U76" s="19" t="n"/>
@@ -4453,7 +4455,7 @@
       </c>
       <c r="Q77" s="19" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-21</t>
         </is>
       </c>
       <c r="R77" s="19" t="inlineStr">
@@ -4493,18 +4495,16 @@
       </c>
       <c r="Q78" s="19" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-12</t>
         </is>
       </c>
       <c r="R78" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
-        </is>
-      </c>
-      <c r="S78" s="19" t="inlineStr">
-        <is>
-          <t>WLS</t>
-        </is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S78" s="19" t="n">
+        <v/>
       </c>
       <c r="T78" s="19" t="n"/>
       <c r="U78" s="19" t="n"/>
@@ -4535,17 +4535,17 @@
       </c>
       <c r="Q79" s="19" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-07</t>
         </is>
       </c>
       <c r="R79" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>AWP</t>
         </is>
       </c>
       <c r="S79" s="19" t="inlineStr">
         <is>
-          <t>WLS</t>
+          <t>JAM</t>
         </is>
       </c>
       <c r="T79" s="19" t="n"/>
@@ -4577,7 +4577,7 @@
       </c>
       <c r="Q80" s="19" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2024-11-03</t>
         </is>
       </c>
       <c r="R80" s="19" t="inlineStr">
@@ -4585,10 +4585,8 @@
           <t>GLO</t>
         </is>
       </c>
-      <c r="S80" s="19" t="inlineStr">
-        <is>
-          <t>JHA</t>
-        </is>
+      <c r="S80" s="19" t="n">
+        <v/>
       </c>
       <c r="T80" s="19" t="n"/>
       <c r="U80" s="19" t="n"/>
@@ -4619,17 +4617,17 @@
       </c>
       <c r="Q81" s="19" t="inlineStr">
         <is>
-          <t>2024-10-16</t>
+          <t>2024-11-03</t>
         </is>
       </c>
       <c r="R81" s="19" t="inlineStr">
         <is>
-          <t>ASM</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S81" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>WLS</t>
         </is>
       </c>
       <c r="T81" s="19" t="n"/>
@@ -4661,16 +4659,18 @@
       </c>
       <c r="Q82" s="19" t="inlineStr">
         <is>
-          <t>2024-10-16</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="R82" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
-        </is>
-      </c>
-      <c r="S82" s="19" t="n">
-        <v/>
+          <t>GLO</t>
+        </is>
+      </c>
+      <c r="S82" s="19" t="inlineStr">
+        <is>
+          <t>WLS</t>
+        </is>
       </c>
       <c r="T82" s="19" t="n"/>
       <c r="U82" s="19" t="n"/>
@@ -4701,17 +4701,17 @@
       </c>
       <c r="Q83" s="19" t="inlineStr">
         <is>
-          <t>2024-10-15</t>
+          <t>2024-10-21</t>
         </is>
       </c>
       <c r="R83" s="19" t="inlineStr">
         <is>
-          <t>JWA</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S83" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>JHA</t>
         </is>
       </c>
       <c r="T83" s="19" t="n"/>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="Q84" s="19" t="inlineStr">
         <is>
-          <t>2024-10-11</t>
+          <t>2024-10-16</t>
         </is>
       </c>
       <c r="R84" s="19" t="inlineStr">
@@ -4753,7 +4753,7 @@
       </c>
       <c r="S84" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="T84" s="19" t="n"/>
@@ -4785,12 +4785,12 @@
       </c>
       <c r="Q85" s="19" t="inlineStr">
         <is>
-          <t>2024-10-05</t>
+          <t>2024-10-16</t>
         </is>
       </c>
       <c r="R85" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>AWP</t>
         </is>
       </c>
       <c r="S85" s="19" t="n">
@@ -4825,16 +4825,18 @@
       </c>
       <c r="Q86" s="19" t="inlineStr">
         <is>
-          <t>2024-10-05</t>
+          <t>2024-10-15</t>
         </is>
       </c>
       <c r="R86" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
-        </is>
-      </c>
-      <c r="S86" s="19" t="n">
-        <v/>
+          <t>JWA</t>
+        </is>
+      </c>
+      <c r="S86" s="19" t="inlineStr">
+        <is>
+          <t>LDE</t>
+        </is>
       </c>
       <c r="T86" s="19" t="n"/>
       <c r="U86" s="19" t="n"/>
@@ -4865,16 +4867,18 @@
       </c>
       <c r="Q87" s="19" t="inlineStr">
         <is>
-          <t>2024-10-04</t>
+          <t>2024-10-11</t>
         </is>
       </c>
       <c r="R87" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
-        </is>
-      </c>
-      <c r="S87" s="19" t="n">
-        <v/>
+          <t>ASM</t>
+        </is>
+      </c>
+      <c r="S87" s="19" t="inlineStr">
+        <is>
+          <t>LDE</t>
+        </is>
       </c>
       <c r="T87" s="19" t="n"/>
       <c r="U87" s="19" t="n"/>
@@ -4905,18 +4909,16 @@
       </c>
       <c r="Q88" s="19" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-05</t>
         </is>
       </c>
       <c r="R88" s="19" t="inlineStr">
         <is>
-          <t>JHA</t>
-        </is>
-      </c>
-      <c r="S88" s="19" t="inlineStr">
-        <is>
-          <t>MIR</t>
-        </is>
+          <t>PRT</t>
+        </is>
+      </c>
+      <c r="S88" s="19" t="n">
+        <v/>
       </c>
       <c r="T88" s="19" t="n"/>
       <c r="U88" s="19" t="n"/>
@@ -4947,12 +4949,12 @@
       </c>
       <c r="Q89" s="19" t="inlineStr">
         <is>
-          <t>2024-09-22</t>
+          <t>2024-10-05</t>
         </is>
       </c>
       <c r="R89" s="19" t="inlineStr">
         <is>
-          <t>TKI</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="S89" s="19" t="n">
@@ -4987,18 +4989,16 @@
       </c>
       <c r="Q90" s="19" t="inlineStr">
         <is>
-          <t>2024-09-12</t>
+          <t>2024-10-04</t>
         </is>
       </c>
       <c r="R90" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
-        </is>
-      </c>
-      <c r="S90" s="19" t="inlineStr">
-        <is>
-          <t>WWH</t>
-        </is>
+          <t>PRT</t>
+        </is>
+      </c>
+      <c r="S90" s="19" t="n">
+        <v/>
       </c>
       <c r="T90" s="19" t="n"/>
       <c r="U90" s="19" t="n"/>
@@ -5029,16 +5029,18 @@
       </c>
       <c r="Q91" s="19" t="inlineStr">
         <is>
-          <t>2024-08-30</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="R91" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
-        </is>
-      </c>
-      <c r="S91" s="19" t="n">
-        <v/>
+          <t>JHA</t>
+        </is>
+      </c>
+      <c r="S91" s="19" t="inlineStr">
+        <is>
+          <t>MIR</t>
+        </is>
       </c>
       <c r="T91" s="19" t="n"/>
       <c r="U91" s="19" t="n"/>
@@ -5069,18 +5071,16 @@
       </c>
       <c r="Q92" s="19" t="inlineStr">
         <is>
-          <t>2024-08-03</t>
+          <t>2024-09-22</t>
         </is>
       </c>
       <c r="R92" s="19" t="inlineStr">
         <is>
-          <t>CSY</t>
-        </is>
-      </c>
-      <c r="S92" s="19" t="inlineStr">
-        <is>
-          <t>PRT</t>
-        </is>
+          <t>TKI</t>
+        </is>
+      </c>
+      <c r="S92" s="19" t="n">
+        <v/>
       </c>
       <c r="T92" s="19" t="n"/>
       <c r="U92" s="19" t="n"/>
@@ -5111,18 +5111,16 @@
       </c>
       <c r="Q93" s="19" t="inlineStr">
         <is>
-          <t>2024-08-02</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="R93" s="19" t="inlineStr">
         <is>
-          <t>JPJ</t>
-        </is>
-      </c>
-      <c r="S93" s="19" t="inlineStr">
-        <is>
-          <t>JYK</t>
-        </is>
+          <t>SMB</t>
+        </is>
+      </c>
+      <c r="S93" s="19" t="n">
+        <v/>
       </c>
       <c r="T93" s="19" t="n"/>
       <c r="U93" s="19" t="n"/>
@@ -5153,17 +5151,17 @@
       </c>
       <c r="Q94" s="19" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-03</t>
         </is>
       </c>
       <c r="R94" s="19" t="inlineStr">
         <is>
-          <t>MBE</t>
+          <t>CSY</t>
         </is>
       </c>
       <c r="S94" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="T94" s="19" t="n"/>
@@ -5195,17 +5193,17 @@
       </c>
       <c r="Q95" s="19" t="inlineStr">
         <is>
-          <t>2024-06-28</t>
+          <t>2024-08-02</t>
         </is>
       </c>
       <c r="R95" s="19" t="inlineStr">
         <is>
-          <t>RTH</t>
+          <t>JPJ</t>
         </is>
       </c>
       <c r="S95" s="19" t="inlineStr">
         <is>
-          <t>RUB</t>
+          <t>JYK</t>
         </is>
       </c>
       <c r="T95" s="19" t="n"/>
@@ -5237,16 +5235,18 @@
       </c>
       <c r="Q96" s="19" t="inlineStr">
         <is>
-          <t>2024-06-28</t>
+          <t>2024-07-01</t>
         </is>
       </c>
       <c r="R96" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
-        </is>
-      </c>
-      <c r="S96" s="19" t="n">
-        <v/>
+          <t>MBE</t>
+        </is>
+      </c>
+      <c r="S96" s="19" t="inlineStr">
+        <is>
+          <t>RJC</t>
+        </is>
       </c>
       <c r="T96" s="19" t="n"/>
       <c r="U96" s="19" t="n"/>
@@ -5277,16 +5277,18 @@
       </c>
       <c r="Q97" s="19" t="inlineStr">
         <is>
-          <t>2024-06-22</t>
+          <t>2024-06-28</t>
         </is>
       </c>
       <c r="R97" s="19" t="inlineStr">
         <is>
-          <t>JPJ</t>
-        </is>
-      </c>
-      <c r="S97" s="19" t="n">
-        <v/>
+          <t>RTH</t>
+        </is>
+      </c>
+      <c r="S97" s="19" t="inlineStr">
+        <is>
+          <t>RUB</t>
+        </is>
       </c>
       <c r="T97" s="19" t="n"/>
       <c r="U97" s="19" t="n"/>
@@ -5317,7 +5319,7 @@
       </c>
       <c r="Q98" s="19" t="inlineStr">
         <is>
-          <t>2024-06-15</t>
+          <t>2024-06-28</t>
         </is>
       </c>
       <c r="R98" s="19" t="inlineStr">
@@ -5357,18 +5359,16 @@
       </c>
       <c r="Q99" s="19" t="inlineStr">
         <is>
-          <t>2024-06-14</t>
+          <t>2024-06-22</t>
         </is>
       </c>
       <c r="R99" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
-        </is>
-      </c>
-      <c r="S99" s="19" t="inlineStr">
-        <is>
-          <t>HAS</t>
-        </is>
+          <t>JPJ</t>
+        </is>
+      </c>
+      <c r="S99" s="19" t="n">
+        <v/>
       </c>
       <c r="T99" s="19" t="n"/>
       <c r="U99" s="19" t="n"/>
@@ -5399,12 +5399,12 @@
       </c>
       <c r="Q100" s="19" t="inlineStr">
         <is>
-          <t>2024-05-24</t>
+          <t>2024-06-15</t>
         </is>
       </c>
       <c r="R100" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S100" s="19" t="n">
@@ -5439,16 +5439,18 @@
       </c>
       <c r="Q101" s="19" t="inlineStr">
         <is>
-          <t>2024-05-19</t>
+          <t>2024-06-14</t>
         </is>
       </c>
       <c r="R101" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S101" s="19" t="n">
-        <v/>
+          <t>CMC</t>
+        </is>
+      </c>
+      <c r="S101" s="19" t="inlineStr">
+        <is>
+          <t>HAS</t>
+        </is>
       </c>
       <c r="T101" s="19" t="n"/>
       <c r="U101" s="19" t="n"/>
@@ -5479,12 +5481,12 @@
       </c>
       <c r="Q102" s="19" t="inlineStr">
         <is>
-          <t>2024-05-18</t>
+          <t>2024-05-24</t>
         </is>
       </c>
       <c r="R102" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="S102" s="19" t="n">
@@ -5519,7 +5521,7 @@
       </c>
       <c r="Q103" s="19" t="inlineStr">
         <is>
-          <t>2024-05-17</t>
+          <t>2024-05-19</t>
         </is>
       </c>
       <c r="R103" s="19" t="inlineStr">
@@ -5559,18 +5561,16 @@
       </c>
       <c r="Q104" s="19" t="inlineStr">
         <is>
-          <t>2024-05-17</t>
+          <t>2024-05-18</t>
         </is>
       </c>
       <c r="R104" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
-        </is>
-      </c>
-      <c r="S104" s="19" t="inlineStr">
-        <is>
-          <t>RTH</t>
-        </is>
+          <t>GLO</t>
+        </is>
+      </c>
+      <c r="S104" s="19" t="n">
+        <v/>
       </c>
       <c r="T104" s="19" t="n"/>
       <c r="U104" s="19" t="n"/>
@@ -5601,16 +5601,18 @@
       </c>
       <c r="Q105" s="19" t="inlineStr">
         <is>
-          <t>2024-05-07</t>
+          <t>2024-05-17</t>
         </is>
       </c>
       <c r="R105" s="19" t="inlineStr">
         <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="S105" s="19" t="n">
-        <v/>
+          <t>LOV</t>
+        </is>
+      </c>
+      <c r="S105" s="19" t="inlineStr">
+        <is>
+          <t>RTH</t>
+        </is>
       </c>
       <c r="T105" s="19" t="n"/>
       <c r="U105" s="19" t="n"/>
@@ -5641,12 +5643,12 @@
       </c>
       <c r="Q106" s="19" t="inlineStr">
         <is>
-          <t>2024-04-20</t>
+          <t>2024-05-17</t>
         </is>
       </c>
       <c r="R106" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S106" s="19" t="n">
@@ -5681,18 +5683,16 @@
       </c>
       <c r="Q107" s="19" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-05-07</t>
         </is>
       </c>
       <c r="R107" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S107" s="19" t="inlineStr">
-        <is>
-          <t>HMK</t>
-        </is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="S107" s="19" t="n">
+        <v/>
       </c>
       <c r="T107" s="19" t="n"/>
       <c r="U107" s="19" t="n"/>
@@ -5723,12 +5723,12 @@
       </c>
       <c r="Q108" s="19" t="inlineStr">
         <is>
-          <t>2024-03-24</t>
+          <t>2024-04-20</t>
         </is>
       </c>
       <c r="R108" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S108" s="19" t="n">
@@ -5763,16 +5763,18 @@
       </c>
       <c r="Q109" s="19" t="inlineStr">
         <is>
-          <t>2024-03-22</t>
+          <t>2024-04-02</t>
         </is>
       </c>
       <c r="R109" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
-        </is>
-      </c>
-      <c r="S109" s="19" t="n">
-        <v/>
+          <t>DDC</t>
+        </is>
+      </c>
+      <c r="S109" s="19" t="inlineStr">
+        <is>
+          <t>HMK</t>
+        </is>
       </c>
       <c r="T109" s="19" t="n"/>
       <c r="U109" s="19" t="n"/>
@@ -5803,12 +5805,12 @@
       </c>
       <c r="Q110" s="19" t="inlineStr">
         <is>
-          <t>2024-03-05</t>
+          <t>2024-03-24</t>
         </is>
       </c>
       <c r="R110" s="19" t="inlineStr">
         <is>
-          <t>JPK</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="S110" s="19" t="n">
@@ -5843,18 +5845,16 @@
       </c>
       <c r="Q111" s="19" t="inlineStr">
         <is>
-          <t>2024-03-03</t>
+          <t>2024-03-22</t>
         </is>
       </c>
       <c r="R111" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
-        </is>
-      </c>
-      <c r="S111" s="19" t="inlineStr">
-        <is>
-          <t>JYK</t>
-        </is>
+          <t>PRT</t>
+        </is>
+      </c>
+      <c r="S111" s="19" t="n">
+        <v/>
       </c>
       <c r="T111" s="19" t="n"/>
       <c r="U111" s="19" t="n"/>
@@ -5885,18 +5885,16 @@
       </c>
       <c r="Q112" s="19" t="inlineStr">
         <is>
-          <t>2024-02-08</t>
+          <t>2024-03-05</t>
         </is>
       </c>
       <c r="R112" s="19" t="inlineStr">
         <is>
-          <t>CSY</t>
-        </is>
-      </c>
-      <c r="S112" s="19" t="inlineStr">
-        <is>
-          <t>PRT</t>
-        </is>
+          <t>JPK</t>
+        </is>
+      </c>
+      <c r="S112" s="19" t="n">
+        <v/>
       </c>
       <c r="T112" s="19" t="n"/>
       <c r="U112" s="19" t="n"/>
@@ -5927,17 +5925,17 @@
       </c>
       <c r="Q113" s="19" t="inlineStr">
         <is>
-          <t>2024-01-26</t>
+          <t>2024-03-03</t>
         </is>
       </c>
       <c r="R113" s="19" t="inlineStr">
         <is>
-          <t>ASM</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S113" s="19" t="inlineStr">
         <is>
-          <t>HEI</t>
+          <t>JYK</t>
         </is>
       </c>
       <c r="T113" s="19" t="n"/>
@@ -5969,17 +5967,17 @@
       </c>
       <c r="Q114" s="19" t="inlineStr">
         <is>
-          <t>2023-12-20</t>
+          <t>2024-02-08</t>
         </is>
       </c>
       <c r="R114" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>CSY</t>
         </is>
       </c>
       <c r="S114" s="19" t="inlineStr">
         <is>
-          <t>YAT</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="T114" s="19" t="n"/>
@@ -6011,17 +6009,17 @@
       </c>
       <c r="Q115" s="19" t="inlineStr">
         <is>
-          <t>2023-11-21</t>
+          <t>2024-01-26</t>
         </is>
       </c>
       <c r="R115" s="19" t="inlineStr">
         <is>
-          <t>JYK</t>
+          <t>ASM</t>
         </is>
       </c>
       <c r="S115" s="19" t="inlineStr">
         <is>
-          <t>WLM</t>
+          <t>HEI</t>
         </is>
       </c>
       <c r="T115" s="19" t="n"/>
@@ -6053,16 +6051,18 @@
       </c>
       <c r="Q116" s="19" t="inlineStr">
         <is>
-          <t>2023-11-20</t>
+          <t>2023-12-20</t>
         </is>
       </c>
       <c r="R116" s="19" t="inlineStr">
         <is>
-          <t>NAY</t>
-        </is>
-      </c>
-      <c r="S116" s="19" t="n">
-        <v/>
+          <t>CMC</t>
+        </is>
+      </c>
+      <c r="S116" s="19" t="inlineStr">
+        <is>
+          <t>YAT</t>
+        </is>
       </c>
       <c r="T116" s="19" t="n"/>
       <c r="U116" s="19" t="n"/>
@@ -6093,12 +6093,12 @@
       </c>
       <c r="Q117" s="19" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>2023-11-20</t>
         </is>
       </c>
       <c r="R117" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
+          <t>NAY</t>
         </is>
       </c>
       <c r="S117" s="19" t="n">
@@ -6173,12 +6173,12 @@
       </c>
       <c r="Q119" s="19" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>2023-11-12</t>
         </is>
       </c>
       <c r="R119" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S119" s="19" t="n">
@@ -6213,12 +6213,12 @@
       </c>
       <c r="Q120" s="19" t="inlineStr">
         <is>
-          <t>2023-10-08</t>
+          <t>2023-11-04</t>
         </is>
       </c>
       <c r="R120" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="S120" s="19" t="n">
@@ -6253,18 +6253,16 @@
       </c>
       <c r="Q121" s="19" t="inlineStr">
         <is>
-          <t>2023-10-06</t>
+          <t>2023-10-08</t>
         </is>
       </c>
       <c r="R121" s="19" t="inlineStr">
         <is>
-          <t>TKI</t>
-        </is>
-      </c>
-      <c r="S121" s="19" t="inlineStr">
-        <is>
-          <t>WLS</t>
-        </is>
+          <t>GLO</t>
+        </is>
+      </c>
+      <c r="S121" s="19" t="n">
+        <v/>
       </c>
       <c r="T121" s="19" t="n"/>
       <c r="U121" s="19" t="n"/>
@@ -6384,12 +6382,12 @@
       </c>
       <c r="R124" s="19" t="inlineStr">
         <is>
-          <t>CWI</t>
+          <t>ASM</t>
         </is>
       </c>
       <c r="S124" s="19" t="inlineStr">
         <is>
-          <t>NAY</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="T124" s="19" t="n"/>

</xml_diff>

<commit_message>
Truly Final Commit (For real this time)
Added caching for the PDF parsing step, which took the most time. Now if the data exists from a previous run, the program will use that instead of re-downloading and re-parsing the PDFs. This should significantly speed up subsequent runs with the same data.

Also fixed a minor issue where whitelisted airports weren't getting green pins.

Should be fully functional and way more efficient.
</commit_message>
<xml_diff>
--- a/wb_list.xlsx
+++ b/wb_list.xlsx
@@ -867,17 +867,17 @@
       </c>
       <c r="Q2" s="19" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="R2" s="19" t="inlineStr">
         <is>
-          <t>CJO</t>
+          <t>JWG</t>
         </is>
       </c>
       <c r="S2" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>RBL</t>
         </is>
       </c>
       <c r="T2" s="19" t="n"/>
@@ -954,17 +954,17 @@
       </c>
       <c r="Q3" s="19" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="R3" s="19" t="inlineStr">
         <is>
-          <t>CJO</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="S3" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="T3" s="19" t="n"/>
@@ -1022,17 +1022,17 @@
       </c>
       <c r="Q4" s="19" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="R4" s="19" t="inlineStr">
         <is>
-          <t>CJO</t>
+          <t>AWP</t>
         </is>
       </c>
       <c r="S4" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="T4" s="19" t="n"/>
@@ -1158,17 +1158,17 @@
       </c>
       <c r="Q6" s="19" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R6" s="19" t="inlineStr">
         <is>
-          <t>HAS</t>
+          <t>CJO</t>
         </is>
       </c>
       <c r="S6" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="T6" s="19" t="n"/>
@@ -1227,17 +1227,17 @@
       </c>
       <c r="Q7" s="19" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R7" s="19" t="inlineStr">
         <is>
-          <t>HAS</t>
+          <t>AFU</t>
         </is>
       </c>
       <c r="S7" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="T7" s="19" t="n"/>
@@ -1301,12 +1301,12 @@
       </c>
       <c r="R8" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
+          <t>HAS</t>
         </is>
       </c>
       <c r="S8" s="19" t="inlineStr">
         <is>
-          <t>JWA</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="T8" s="19" t="n"/>
@@ -1365,11 +1365,13 @@
       </c>
       <c r="R9" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S9" s="19" t="n">
-        <v/>
+          <t>HAS</t>
+        </is>
+      </c>
+      <c r="S9" s="19" t="inlineStr">
+        <is>
+          <t>WSM</t>
+        </is>
       </c>
       <c r="T9" s="19" t="n"/>
       <c r="U9" s="19" t="n"/>
@@ -1424,11 +1426,13 @@
       </c>
       <c r="R10" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S10" s="19" t="n">
-        <v/>
+          <t>DDC</t>
+        </is>
+      </c>
+      <c r="S10" s="19" t="inlineStr">
+        <is>
+          <t>JWA</t>
+        </is>
       </c>
       <c r="T10" s="19" t="n"/>
       <c r="U10" s="19" t="n"/>
@@ -1479,13 +1483,11 @@
       </c>
       <c r="R11" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S11" s="19" t="inlineStr">
-        <is>
-          <t>RBL</t>
-        </is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S11" s="19" t="n">
+        <v/>
       </c>
       <c r="T11" s="19" t="n"/>
       <c r="U11" s="19" t="n"/>
@@ -1537,13 +1539,11 @@
       </c>
       <c r="R12" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S12" s="19" t="inlineStr">
-        <is>
-          <t>RBL</t>
-        </is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S12" s="19" t="n">
+        <v/>
       </c>
       <c r="T12" s="19" t="n"/>
       <c r="U12" s="19" t="n"/>
@@ -1594,17 +1594,17 @@
       </c>
       <c r="Q13" s="19" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R13" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S13" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>RBL</t>
         </is>
       </c>
       <c r="T13" s="19" t="n"/>
@@ -1651,17 +1651,17 @@
       </c>
       <c r="Q14" s="19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R14" s="19" t="inlineStr">
         <is>
-          <t>JWG</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S14" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>RBL</t>
         </is>
       </c>
       <c r="T14" s="19" t="n"/>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="Q15" s="19" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="R15" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>CBI</t>
         </is>
       </c>
       <c r="S15" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="T15" s="19" t="n"/>
@@ -1757,12 +1757,12 @@
       </c>
       <c r="Q16" s="19" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="R16" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="S16" s="19" t="n">
@@ -1809,17 +1809,17 @@
       </c>
       <c r="Q17" s="19" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="R17" s="19" t="inlineStr">
         <is>
-          <t>JPJ</t>
+          <t>AWP</t>
         </is>
       </c>
       <c r="S17" s="19" t="inlineStr">
         <is>
-          <t>WLS</t>
+          <t>JWG</t>
         </is>
       </c>
       <c r="T17" s="19" t="n"/>
@@ -1867,17 +1867,17 @@
       </c>
       <c r="Q18" s="19" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="R18" s="19" t="inlineStr">
         <is>
-          <t>HMK</t>
+          <t>JPJ</t>
         </is>
       </c>
       <c r="S18" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>WLS</t>
         </is>
       </c>
       <c r="T18" s="19" t="n"/>
@@ -1920,17 +1920,17 @@
       </c>
       <c r="Q19" s="19" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="R19" s="19" t="inlineStr">
         <is>
-          <t>ADO</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S19" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>JAM</t>
         </is>
       </c>
       <c r="T19" s="19" t="n"/>
@@ -1973,17 +1973,17 @@
       </c>
       <c r="Q20" s="19" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="R20" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>ADO</t>
         </is>
       </c>
       <c r="S20" s="19" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="T20" s="19" t="n"/>
@@ -2027,17 +2027,17 @@
       </c>
       <c r="Q21" s="19" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="R21" s="19" t="inlineStr">
         <is>
-          <t>JWA</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S21" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="T21" s="19" t="n"/>
@@ -2085,17 +2085,17 @@
       </c>
       <c r="Q22" s="19" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="R22" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>JWA</t>
         </is>
       </c>
       <c r="S22" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="T22" s="19" t="n"/>
@@ -2192,12 +2192,12 @@
       </c>
       <c r="Q24" s="19" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="R24" s="19" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>CBI</t>
         </is>
       </c>
       <c r="S24" s="19" t="inlineStr">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="Q25" s="19" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="R25" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="S25" s="19" t="inlineStr">
         <is>
-          <t>HMK</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="T25" s="19" t="n"/>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="Q26" s="19" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="R26" s="19" t="inlineStr">
         <is>
-          <t>JMO</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S26" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>HMK</t>
         </is>
       </c>
       <c r="T26" s="19" t="n"/>
@@ -2357,17 +2357,17 @@
       </c>
       <c r="Q27" s="19" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="R27" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>JMO</t>
         </is>
       </c>
       <c r="S27" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="T27" s="19" t="n"/>
@@ -2411,17 +2411,17 @@
       </c>
       <c r="Q28" s="19" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="R28" s="19" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S28" s="19" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>LOV</t>
         </is>
       </c>
       <c r="T28" s="19" t="n"/>
@@ -2470,12 +2470,12 @@
       </c>
       <c r="R29" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="S29" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>TIN</t>
         </is>
       </c>
       <c r="T29" s="19" t="n"/>
@@ -2519,16 +2519,18 @@
       </c>
       <c r="Q30" s="19" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="R30" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="S30" s="19" t="n">
-        <v/>
+          <t>CBI</t>
+        </is>
+      </c>
+      <c r="S30" s="19" t="inlineStr">
+        <is>
+          <t>SMB</t>
+        </is>
       </c>
       <c r="T30" s="19" t="n"/>
       <c r="U30" s="19" t="n"/>
@@ -2576,13 +2578,11 @@
       </c>
       <c r="R31" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S31" s="19" t="inlineStr">
-        <is>
-          <t>FRU</t>
-        </is>
+          <t>MAN</t>
+        </is>
+      </c>
+      <c r="S31" s="19" t="n">
+        <v/>
       </c>
       <c r="T31" s="19" t="n"/>
       <c r="U31" s="19" t="n"/>
@@ -2613,17 +2613,17 @@
       </c>
       <c r="Q32" s="19" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-19</t>
         </is>
       </c>
       <c r="R32" s="19" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S32" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="T32" s="19" t="n"/>
@@ -2655,17 +2655,17 @@
       </c>
       <c r="Q33" s="19" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-14</t>
         </is>
       </c>
       <c r="R33" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>LAO</t>
         </is>
       </c>
       <c r="S33" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="T33" s="19" t="n"/>
@@ -6508,7 +6508,7 @@
       </c>
       <c r="R127" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>DSJ</t>
         </is>
       </c>
       <c r="S127" s="19" t="n">
@@ -6796,11 +6796,13 @@
       </c>
       <c r="R134" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
-        </is>
-      </c>
-      <c r="S134" s="19" t="n">
-        <v/>
+          <t>JHA</t>
+        </is>
+      </c>
+      <c r="S134" s="19" t="inlineStr">
+        <is>
+          <t>WWH</t>
+        </is>
       </c>
       <c r="T134" s="19" t="n"/>
       <c r="U134" s="19" t="n"/>
@@ -6836,13 +6838,11 @@
       </c>
       <c r="R135" s="19" t="inlineStr">
         <is>
-          <t>JHA</t>
-        </is>
-      </c>
-      <c r="S135" s="19" t="inlineStr">
-        <is>
-          <t>WWH</t>
-        </is>
+          <t>CMC</t>
+        </is>
+      </c>
+      <c r="S135" s="19" t="n">
+        <v/>
       </c>
       <c r="T135" s="19" t="n"/>
       <c r="U135" s="19" t="n"/>

</xml_diff>